<commit_message>
Migration to Model , Import from Excel File
</commit_message>
<xml_diff>
--- a/hrms-client/SALARY  Format.xlsx
+++ b/hrms-client/SALARY  Format.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Personal\HRMS\hrms\hrms-client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7950" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10395" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Master" sheetId="9" r:id="rId1"/>
-    <sheet name="Salary Sheet" sheetId="1" r:id="rId2"/>
-    <sheet name="Salary Acknowledgement Sheet" sheetId="3" r:id="rId3"/>
-    <sheet name="Payslip" sheetId="5" r:id="rId4"/>
-    <sheet name="EPF" sheetId="10" r:id="rId5"/>
-    <sheet name="ESI" sheetId="11" r:id="rId6"/>
+    <sheet name="EmployeePayrollMaster" sheetId="12" r:id="rId2"/>
+    <sheet name="Salary Sheet" sheetId="1" r:id="rId3"/>
+    <sheet name="Salary Acknowledgement Sheet" sheetId="3" r:id="rId4"/>
+    <sheet name="Payslip" sheetId="5" r:id="rId5"/>
+    <sheet name="EPF" sheetId="10" r:id="rId6"/>
+    <sheet name="ESI" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Master'!$A$2:$AF$17</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="128">
   <si>
     <t>Sl.No</t>
   </si>
@@ -464,11 +470,26 @@
       <t>( Format DD/MM/YYYY  or DD-MM-YYYY)</t>
     </r>
   </si>
+  <si>
+    <t>Basic Pay</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Dearness Allowance</t>
+  </si>
+  <si>
+    <t>House Rent Allowance</t>
+  </si>
+  <si>
+    <t>City Compensation Allowance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
@@ -1445,78 +1466,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1570,6 +1519,78 @@
     </xf>
     <xf numFmtId="49" fontId="27" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1582,6 +1603,14 @@
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1628,7 +1657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1660,9 +1689,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1694,6 +1724,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1869,11 +1900,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1899,39 +1930,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="27">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="156" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
-      <c r="P1" s="137"/>
-      <c r="Q1" s="137"/>
-      <c r="R1" s="137"/>
-      <c r="S1" s="137"/>
-      <c r="T1" s="137"/>
-      <c r="U1" s="137"/>
-      <c r="V1" s="137"/>
-      <c r="W1" s="137"/>
-      <c r="X1" s="137"/>
-      <c r="Y1" s="137"/>
-      <c r="Z1" s="137"/>
-      <c r="AA1" s="137"/>
-      <c r="AB1" s="137"/>
-      <c r="AC1" s="137"/>
-      <c r="AD1" s="137"/>
-      <c r="AE1" s="138"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="157"/>
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="158"/>
     </row>
     <row r="2" spans="1:32" ht="36">
       <c r="A2" s="49" t="s">
@@ -2253,24 +2284,24 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="131"/>
-      <c r="D9" s="160"/>
+      <c r="D9" s="136"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="161"/>
-      <c r="H9" s="162"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="138"/>
       <c r="I9" s="48"/>
       <c r="J9" s="45"/>
-      <c r="K9" s="163"/>
-      <c r="L9" s="164"/>
-      <c r="M9" s="165"/>
-      <c r="N9" s="165"/>
-      <c r="O9" s="166"/>
-      <c r="P9" s="166"/>
-      <c r="Q9" s="167"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="140"/>
+      <c r="M9" s="141"/>
+      <c r="N9" s="141"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="142"/>
+      <c r="Q9" s="143"/>
       <c r="R9" s="130"/>
       <c r="S9" s="131"/>
-      <c r="T9" s="168"/>
-      <c r="U9" s="169"/>
+      <c r="T9" s="144"/>
+      <c r="U9" s="145"/>
       <c r="V9" s="131"/>
       <c r="W9" s="131"/>
       <c r="X9" s="131"/>
@@ -2289,24 +2320,24 @@
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="131"/>
-      <c r="D10" s="160"/>
+      <c r="D10" s="136"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="160"/>
+      <c r="F10" s="136"/>
       <c r="G10" s="48"/>
-      <c r="H10" s="162"/>
+      <c r="H10" s="138"/>
       <c r="I10" s="48"/>
       <c r="J10" s="131"/>
-      <c r="K10" s="163"/>
-      <c r="L10" s="164"/>
-      <c r="M10" s="165"/>
-      <c r="N10" s="165"/>
-      <c r="O10" s="166"/>
-      <c r="P10" s="166"/>
-      <c r="Q10" s="167"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="140"/>
+      <c r="M10" s="141"/>
+      <c r="N10" s="141"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="143"/>
       <c r="R10" s="130"/>
       <c r="S10" s="131"/>
-      <c r="T10" s="168"/>
-      <c r="U10" s="169"/>
+      <c r="T10" s="144"/>
+      <c r="U10" s="145"/>
       <c r="V10" s="131"/>
       <c r="W10" s="131"/>
       <c r="X10" s="131"/>
@@ -2325,24 +2356,24 @@
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="131"/>
-      <c r="D11" s="160"/>
+      <c r="D11" s="136"/>
       <c r="E11" s="46"/>
-      <c r="F11" s="160"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="162"/>
+      <c r="H11" s="138"/>
       <c r="I11" s="48"/>
       <c r="J11" s="131"/>
-      <c r="K11" s="163"/>
-      <c r="L11" s="164"/>
-      <c r="M11" s="165"/>
-      <c r="N11" s="165"/>
-      <c r="O11" s="166"/>
-      <c r="P11" s="166"/>
-      <c r="Q11" s="167"/>
+      <c r="K11" s="139"/>
+      <c r="L11" s="140"/>
+      <c r="M11" s="141"/>
+      <c r="N11" s="141"/>
+      <c r="O11" s="142"/>
+      <c r="P11" s="142"/>
+      <c r="Q11" s="143"/>
       <c r="R11" s="130"/>
       <c r="S11" s="131"/>
-      <c r="T11" s="168"/>
-      <c r="U11" s="169"/>
+      <c r="T11" s="144"/>
+      <c r="U11" s="145"/>
       <c r="V11" s="131"/>
       <c r="W11" s="131"/>
       <c r="X11" s="131"/>
@@ -2361,24 +2392,24 @@
       </c>
       <c r="B12" s="43"/>
       <c r="C12" s="131"/>
-      <c r="D12" s="160"/>
+      <c r="D12" s="136"/>
       <c r="E12" s="46"/>
-      <c r="F12" s="160"/>
+      <c r="F12" s="136"/>
       <c r="G12" s="48"/>
-      <c r="H12" s="162"/>
+      <c r="H12" s="138"/>
       <c r="I12" s="48"/>
       <c r="J12" s="131"/>
-      <c r="K12" s="163"/>
-      <c r="L12" s="164"/>
-      <c r="M12" s="165"/>
-      <c r="N12" s="165"/>
-      <c r="O12" s="166"/>
-      <c r="P12" s="166"/>
-      <c r="Q12" s="167"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="141"/>
+      <c r="N12" s="141"/>
+      <c r="O12" s="142"/>
+      <c r="P12" s="142"/>
+      <c r="Q12" s="143"/>
       <c r="R12" s="130"/>
       <c r="S12" s="131"/>
-      <c r="T12" s="168"/>
-      <c r="U12" s="169"/>
+      <c r="T12" s="144"/>
+      <c r="U12" s="145"/>
       <c r="V12" s="131"/>
       <c r="W12" s="131"/>
       <c r="X12" s="131"/>
@@ -2476,13 +2507,13 @@
       <c r="H15" s="42"/>
       <c r="I15" s="48"/>
       <c r="J15" s="42"/>
-      <c r="K15" s="170"/>
+      <c r="K15" s="146"/>
       <c r="L15" s="106"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
       <c r="O15" s="106"/>
       <c r="P15" s="106"/>
-      <c r="Q15" s="171"/>
+      <c r="Q15" s="147"/>
       <c r="R15" s="134"/>
       <c r="S15" s="106"/>
       <c r="T15" s="42"/>
@@ -2512,13 +2543,13 @@
       <c r="H16" s="42"/>
       <c r="I16" s="48"/>
       <c r="J16" s="42"/>
-      <c r="K16" s="170"/>
+      <c r="K16" s="146"/>
       <c r="L16" s="106"/>
       <c r="M16" s="106"/>
       <c r="N16" s="106"/>
       <c r="O16" s="106"/>
       <c r="P16" s="106"/>
-      <c r="Q16" s="171"/>
+      <c r="Q16" s="147"/>
       <c r="R16" s="134"/>
       <c r="S16" s="106"/>
       <c r="T16" s="42"/>
@@ -2548,7 +2579,7 @@
       <c r="H17" s="52"/>
       <c r="I17" s="48"/>
       <c r="J17" s="133"/>
-      <c r="K17" s="172"/>
+      <c r="K17" s="148"/>
       <c r="L17" s="51"/>
       <c r="M17" s="51"/>
       <c r="N17" s="51"/>
@@ -2572,9 +2603,7 @@
       <c r="AF17" s="51"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AF17">
-    <filterColumn colId="8"/>
-  </autoFilter>
+  <autoFilter ref="A2:AF17"/>
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
@@ -2592,11 +2621,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2632,49 +2724,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="27">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="159" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
-      <c r="U1" s="139"/>
-      <c r="V1" s="139"/>
-      <c r="W1" s="139"/>
-      <c r="X1" s="139"/>
-      <c r="Y1" s="139"/>
-      <c r="Z1" s="139"/>
-      <c r="AA1" s="139"/>
-      <c r="AB1" s="139"/>
-      <c r="AC1" s="139"/>
-      <c r="AD1" s="139"/>
-      <c r="AE1" s="139"/>
-      <c r="AF1" s="139"/>
-      <c r="AG1" s="139"/>
-      <c r="AH1" s="139"/>
-      <c r="AI1" s="139"/>
-      <c r="AJ1" s="139"/>
-      <c r="AK1" s="139"/>
-      <c r="AL1" s="139"/>
-      <c r="AM1" s="139"/>
-      <c r="AN1" s="139"/>
-      <c r="AO1" s="139"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
+      <c r="O1" s="159"/>
+      <c r="P1" s="159"/>
+      <c r="Q1" s="159"/>
+      <c r="R1" s="159"/>
+      <c r="S1" s="159"/>
+      <c r="T1" s="159"/>
+      <c r="U1" s="159"/>
+      <c r="V1" s="159"/>
+      <c r="W1" s="159"/>
+      <c r="X1" s="159"/>
+      <c r="Y1" s="159"/>
+      <c r="Z1" s="159"/>
+      <c r="AA1" s="159"/>
+      <c r="AB1" s="159"/>
+      <c r="AC1" s="159"/>
+      <c r="AD1" s="159"/>
+      <c r="AE1" s="159"/>
+      <c r="AF1" s="159"/>
+      <c r="AG1" s="159"/>
+      <c r="AH1" s="159"/>
+      <c r="AI1" s="159"/>
+      <c r="AJ1" s="159"/>
+      <c r="AK1" s="159"/>
+      <c r="AL1" s="159"/>
+      <c r="AM1" s="159"/>
+      <c r="AN1" s="159"/>
+      <c r="AO1" s="159"/>
     </row>
     <row r="2" spans="1:47" s="1" customFormat="1" ht="60">
       <c r="A2" s="91" t="s">
@@ -2837,15 +2929,15 @@
         <v>2158</v>
       </c>
       <c r="O3" s="58">
-        <f t="shared" ref="O3:O10" si="0">ROUND(M3/30*I3,0)</f>
+        <f t="shared" ref="O3" si="0">ROUND(M3/30*I3,0)</f>
         <v>9120</v>
       </c>
       <c r="P3" s="58">
-        <f t="shared" ref="P3:P10" si="1">ROUND(N3/30*I3,0)</f>
+        <f t="shared" ref="P3" si="1">ROUND(N3/30*I3,0)</f>
         <v>2158</v>
       </c>
       <c r="Q3" s="58">
-        <f t="shared" ref="Q3:Q12" si="2">ROUND(O3+P3,0)</f>
+        <f t="shared" ref="Q3" si="2">ROUND(O3+P3,0)</f>
         <v>11278</v>
       </c>
       <c r="R3" s="58">
@@ -2858,11 +2950,11 @@
         <v>1948</v>
       </c>
       <c r="U3" s="58">
-        <f t="shared" ref="U3:U12" si="3">ROUND(R3/30*I3,0)</f>
+        <f t="shared" ref="U3" si="3">ROUND(R3/30*I3,0)</f>
         <v>1450</v>
       </c>
       <c r="V3" s="58">
-        <f t="shared" ref="V3:V12" si="4">ROUND(S3/30*I3,0)</f>
+        <f t="shared" ref="V3" si="4">ROUND(S3/30*I3,0)</f>
         <v>200</v>
       </c>
       <c r="W3" s="58">
@@ -2878,7 +2970,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="58">
-        <f t="shared" ref="AA3:AA12" si="5">ROUND(T3/30*I3,0)</f>
+        <f t="shared" ref="AA3" si="5">ROUND(T3/30*I3,0)</f>
         <v>1948</v>
       </c>
       <c r="AB3" s="58">
@@ -2889,11 +2981,11 @@
         <v>14876</v>
       </c>
       <c r="AD3" s="58">
-        <f t="shared" ref="AD3:AD7" si="6">ROUND(Q3*10%,0)</f>
+        <f t="shared" ref="AD3" si="6">ROUND(Q3*10%,0)</f>
         <v>1128</v>
       </c>
       <c r="AE3" s="58">
-        <f t="shared" ref="AE3:AE8" si="7">ROUND(Q3*0.75%,0)</f>
+        <f t="shared" ref="AE3" si="7">ROUND(Q3*0.75%,0)</f>
         <v>85</v>
       </c>
       <c r="AF3" s="58">
@@ -2915,11 +3007,11 @@
         <v>0</v>
       </c>
       <c r="AL3" s="58">
-        <f t="shared" ref="AL3:AL8" si="8">AD3+AE3+AK3+AJ3+AI3+AH3+AG3+AF3</f>
+        <f t="shared" ref="AL3" si="8">AD3+AE3+AK3+AJ3+AI3+AH3+AG3+AF3</f>
         <v>1213</v>
       </c>
       <c r="AM3" s="58">
-        <f t="shared" ref="AM3:AM16" si="9">AC3-AD3-AE3-AF3-AG3-AH3-AI3-AJ3-AK3</f>
+        <f t="shared" ref="AM3" si="9">AC3-AD3-AE3-AF3-AG3-AH3-AI3-AJ3-AK3</f>
         <v>13663</v>
       </c>
       <c r="AN3" s="99" t="s">
@@ -3574,20 +3666,20 @@
       <c r="AU16" s="2"/>
     </row>
     <row r="17" spans="1:41" s="11" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
-      <c r="E17" s="141"/>
-      <c r="F17" s="141"/>
-      <c r="G17" s="141"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="141"/>
-      <c r="K17" s="141"/>
-      <c r="L17" s="141"/>
+      <c r="B17" s="161"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="161"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
+      <c r="J17" s="161"/>
+      <c r="K17" s="161"/>
+      <c r="L17" s="161"/>
       <c r="M17" s="87">
         <f t="shared" ref="M17:AM17" si="10">SUM(M3:M16)</f>
         <v>9120</v>
@@ -3795,12 +3887,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3830,30 +3922,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="25.5">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="162" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
-      <c r="Q1" s="143"/>
-      <c r="R1" s="143"/>
-      <c r="S1" s="143"/>
-      <c r="T1" s="143"/>
-      <c r="U1" s="143"/>
-      <c r="V1" s="144"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="164"/>
     </row>
     <row r="2" spans="1:25" ht="30">
       <c r="A2" s="107" t="s">
@@ -4485,11 +4577,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
@@ -4506,46 +4598,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="179"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="147"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="175"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="176"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="150"/>
-      <c r="B4" s="151"/>
-      <c r="C4" s="151"/>
-      <c r="D4" s="152"/>
+      <c r="A4" s="176"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="167"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="153" t="s">
+      <c r="A5" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="155"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="172"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="151"/>
-      <c r="C6" s="151"/>
-      <c r="D6" s="152"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="167"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="14" t="s">
@@ -4667,47 +4759,47 @@
       <c r="A18" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="145">
+      <c r="B18" s="168">
         <f>B17-D17</f>
         <v>0</v>
       </c>
-      <c r="C18" s="145"/>
-      <c r="D18" s="146"/>
+      <c r="C18" s="168"/>
+      <c r="D18" s="169"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="21" spans="1:4">
-      <c r="A21" s="147"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149"/>
+      <c r="A21" s="173"/>
+      <c r="B21" s="174"/>
+      <c r="C21" s="174"/>
+      <c r="D21" s="175"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="151"/>
-      <c r="D22" s="152"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="166"/>
+      <c r="D22" s="167"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="150"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="152"/>
+      <c r="A23" s="176"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="166"/>
+      <c r="D23" s="167"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="153" t="s">
+      <c r="A24" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="154"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="155"/>
+      <c r="B24" s="171"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="172"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="151"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="152"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="166"/>
+      <c r="D25" s="167"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="14" t="s">
@@ -4829,47 +4921,47 @@
       <c r="A37" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="145">
+      <c r="B37" s="168">
         <f>B36-D36</f>
         <v>0</v>
       </c>
-      <c r="C37" s="145"/>
-      <c r="D37" s="146"/>
+      <c r="C37" s="168"/>
+      <c r="D37" s="169"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="40" spans="1:4">
-      <c r="A40" s="147"/>
-      <c r="B40" s="148"/>
-      <c r="C40" s="148"/>
-      <c r="D40" s="149"/>
+      <c r="A40" s="173"/>
+      <c r="B40" s="174"/>
+      <c r="C40" s="174"/>
+      <c r="D40" s="175"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="150"/>
-      <c r="B41" s="151"/>
-      <c r="C41" s="151"/>
-      <c r="D41" s="152"/>
+      <c r="A41" s="176"/>
+      <c r="B41" s="166"/>
+      <c r="C41" s="166"/>
+      <c r="D41" s="167"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="150"/>
-      <c r="B42" s="151"/>
-      <c r="C42" s="151"/>
-      <c r="D42" s="152"/>
+      <c r="A42" s="176"/>
+      <c r="B42" s="166"/>
+      <c r="C42" s="166"/>
+      <c r="D42" s="167"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="153" t="s">
+      <c r="A43" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="154"/>
-      <c r="C43" s="154"/>
-      <c r="D43" s="155"/>
+      <c r="B43" s="171"/>
+      <c r="C43" s="171"/>
+      <c r="D43" s="172"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="156" t="s">
+      <c r="A44" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="151"/>
-      <c r="C44" s="151"/>
-      <c r="D44" s="152"/>
+      <c r="B44" s="166"/>
+      <c r="C44" s="166"/>
+      <c r="D44" s="167"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="14" t="s">
@@ -4991,47 +5083,47 @@
       <c r="A56" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="145">
+      <c r="B56" s="168">
         <f>B55-D55</f>
         <v>0</v>
       </c>
-      <c r="C56" s="145"/>
-      <c r="D56" s="146"/>
+      <c r="C56" s="168"/>
+      <c r="D56" s="169"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="59" spans="1:4">
-      <c r="A59" s="147"/>
-      <c r="B59" s="148"/>
-      <c r="C59" s="148"/>
-      <c r="D59" s="149"/>
+      <c r="A59" s="173"/>
+      <c r="B59" s="174"/>
+      <c r="C59" s="174"/>
+      <c r="D59" s="175"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="150"/>
-      <c r="B60" s="151"/>
-      <c r="C60" s="151"/>
-      <c r="D60" s="152"/>
+      <c r="A60" s="176"/>
+      <c r="B60" s="166"/>
+      <c r="C60" s="166"/>
+      <c r="D60" s="167"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="150"/>
-      <c r="B61" s="151"/>
-      <c r="C61" s="151"/>
-      <c r="D61" s="152"/>
+      <c r="A61" s="176"/>
+      <c r="B61" s="166"/>
+      <c r="C61" s="166"/>
+      <c r="D61" s="167"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="153" t="s">
+      <c r="A62" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B62" s="154"/>
-      <c r="C62" s="154"/>
-      <c r="D62" s="155"/>
+      <c r="B62" s="171"/>
+      <c r="C62" s="171"/>
+      <c r="D62" s="172"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="156" t="s">
+      <c r="A63" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="151"/>
-      <c r="C63" s="151"/>
-      <c r="D63" s="152"/>
+      <c r="B63" s="166"/>
+      <c r="C63" s="166"/>
+      <c r="D63" s="167"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="14" t="s">
@@ -5153,47 +5245,47 @@
       <c r="A75" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="145">
+      <c r="B75" s="168">
         <f>B74-D74</f>
         <v>0</v>
       </c>
-      <c r="C75" s="145"/>
-      <c r="D75" s="146"/>
+      <c r="C75" s="168"/>
+      <c r="D75" s="169"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="78" spans="1:4">
-      <c r="A78" s="147"/>
-      <c r="B78" s="148"/>
-      <c r="C78" s="148"/>
-      <c r="D78" s="149"/>
+      <c r="A78" s="173"/>
+      <c r="B78" s="174"/>
+      <c r="C78" s="174"/>
+      <c r="D78" s="175"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="150"/>
-      <c r="B79" s="151"/>
-      <c r="C79" s="151"/>
-      <c r="D79" s="152"/>
+      <c r="A79" s="176"/>
+      <c r="B79" s="166"/>
+      <c r="C79" s="166"/>
+      <c r="D79" s="167"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="150"/>
-      <c r="B80" s="151"/>
-      <c r="C80" s="151"/>
-      <c r="D80" s="152"/>
+      <c r="A80" s="176"/>
+      <c r="B80" s="166"/>
+      <c r="C80" s="166"/>
+      <c r="D80" s="167"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="153" t="s">
+      <c r="A81" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="154"/>
-      <c r="C81" s="154"/>
-      <c r="D81" s="155"/>
+      <c r="B81" s="171"/>
+      <c r="C81" s="171"/>
+      <c r="D81" s="172"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="156" t="s">
+      <c r="A82" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B82" s="151"/>
-      <c r="C82" s="151"/>
-      <c r="D82" s="152"/>
+      <c r="B82" s="166"/>
+      <c r="C82" s="166"/>
+      <c r="D82" s="167"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="14" t="s">
@@ -5315,47 +5407,47 @@
       <c r="A94" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B94" s="145">
+      <c r="B94" s="168">
         <f>B93-D93</f>
         <v>0</v>
       </c>
-      <c r="C94" s="145"/>
-      <c r="D94" s="146"/>
+      <c r="C94" s="168"/>
+      <c r="D94" s="169"/>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="97" spans="1:4">
-      <c r="A97" s="147"/>
-      <c r="B97" s="148"/>
-      <c r="C97" s="148"/>
-      <c r="D97" s="149"/>
+      <c r="A97" s="173"/>
+      <c r="B97" s="174"/>
+      <c r="C97" s="174"/>
+      <c r="D97" s="175"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="150"/>
-      <c r="B98" s="151"/>
-      <c r="C98" s="151"/>
-      <c r="D98" s="152"/>
+      <c r="A98" s="176"/>
+      <c r="B98" s="166"/>
+      <c r="C98" s="166"/>
+      <c r="D98" s="167"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="150"/>
-      <c r="B99" s="151"/>
-      <c r="C99" s="151"/>
-      <c r="D99" s="152"/>
+      <c r="A99" s="176"/>
+      <c r="B99" s="166"/>
+      <c r="C99" s="166"/>
+      <c r="D99" s="167"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="153" t="s">
+      <c r="A100" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="154"/>
-      <c r="C100" s="154"/>
-      <c r="D100" s="155"/>
+      <c r="B100" s="171"/>
+      <c r="C100" s="171"/>
+      <c r="D100" s="172"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="156" t="s">
+      <c r="A101" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B101" s="151"/>
-      <c r="C101" s="151"/>
-      <c r="D101" s="152"/>
+      <c r="B101" s="166"/>
+      <c r="C101" s="166"/>
+      <c r="D101" s="167"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="14" t="s">
@@ -5477,47 +5569,47 @@
       <c r="A113" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B113" s="145">
+      <c r="B113" s="168">
         <f>B112-D112</f>
         <v>0</v>
       </c>
-      <c r="C113" s="145"/>
-      <c r="D113" s="146"/>
+      <c r="C113" s="168"/>
+      <c r="D113" s="169"/>
     </row>
     <row r="115" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="116" spans="1:4">
-      <c r="A116" s="147"/>
-      <c r="B116" s="148"/>
-      <c r="C116" s="148"/>
-      <c r="D116" s="149"/>
+      <c r="A116" s="173"/>
+      <c r="B116" s="174"/>
+      <c r="C116" s="174"/>
+      <c r="D116" s="175"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="150"/>
-      <c r="B117" s="151"/>
-      <c r="C117" s="151"/>
-      <c r="D117" s="152"/>
+      <c r="A117" s="176"/>
+      <c r="B117" s="166"/>
+      <c r="C117" s="166"/>
+      <c r="D117" s="167"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="150"/>
-      <c r="B118" s="151"/>
-      <c r="C118" s="151"/>
-      <c r="D118" s="152"/>
+      <c r="A118" s="176"/>
+      <c r="B118" s="166"/>
+      <c r="C118" s="166"/>
+      <c r="D118" s="167"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="153" t="s">
+      <c r="A119" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="B119" s="154"/>
-      <c r="C119" s="154"/>
-      <c r="D119" s="155"/>
+      <c r="B119" s="171"/>
+      <c r="C119" s="171"/>
+      <c r="D119" s="172"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="156" t="s">
+      <c r="A120" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B120" s="151"/>
-      <c r="C120" s="151"/>
-      <c r="D120" s="152"/>
+      <c r="B120" s="166"/>
+      <c r="C120" s="166"/>
+      <c r="D120" s="167"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="14" t="s">
@@ -5639,20 +5731,38 @@
       <c r="A132" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B132" s="145">
+      <c r="B132" s="168">
         <f>B131-D131</f>
         <v>0</v>
       </c>
-      <c r="C132" s="145"/>
-      <c r="D132" s="146"/>
+      <c r="C132" s="168"/>
+      <c r="D132" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
@@ -5665,43 +5775,25 @@
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="B113:D113"/>
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A118:D118"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="B132:D132"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5720,37 +5812,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="149" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="149" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="149" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="173" t="s">
+      <c r="D1" s="149" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="173" t="s">
+      <c r="E1" s="149" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="173" t="s">
+      <c r="F1" s="149" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="173" t="s">
+      <c r="G1" s="149" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="173" t="s">
+      <c r="H1" s="149" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="173" t="s">
+      <c r="I1" s="149" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="173" t="s">
+      <c r="J1" s="149" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="173" t="s">
+      <c r="K1" s="149" t="s">
         <v>116</v>
       </c>
     </row>
@@ -6600,42 +6692,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="175" customWidth="1"/>
-    <col min="2" max="2" width="24" style="175" customWidth="1"/>
-    <col min="3" max="3" width="20" style="176" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="176" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="176" customWidth="1"/>
-    <col min="6" max="6" width="19" style="175" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="174"/>
+    <col min="1" max="1" width="24.28515625" style="151" customWidth="1"/>
+    <col min="2" max="2" width="24" style="151" customWidth="1"/>
+    <col min="3" max="3" width="20" style="152" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="152" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="152" customWidth="1"/>
+    <col min="6" max="6" width="19" style="151" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="150"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="178" customFormat="1" ht="66" customHeight="1">
-      <c r="A1" s="177" t="s">
+    <row r="1" spans="1:7" s="154" customFormat="1" ht="66" customHeight="1">
+      <c r="A1" s="153" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="177" t="s">
+      <c r="B1" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="177" t="s">
+      <c r="C1" s="153" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="177" t="s">
+      <c r="D1" s="153" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="179" t="s">
+      <c r="E1" s="155" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="177" t="s">
+      <c r="F1" s="153" t="s">
         <v>122</v>
       </c>
       <c r="G1" s="3"/>

</xml_diff>